<commit_message>
add new file named push management
</commit_message>
<xml_diff>
--- a/admin_panel/push_management/image_url.xlsx
+++ b/admin_panel/push_management/image_url.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\admin_panel\push_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D648E7C-BB31-4A15-8A05-CB1E2A4561AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB177D-5C6F-4C96-BA3E-FCB5EB175976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -169,14 +169,6 @@
     <t>enter text and navigate through the input field using the tab key.</t>
   </si>
   <si>
-    <t>1. go to  google and search https://adminportal.symlexvpn.com/vpnadmin/index.php/login/index
-2. login with proper credentials
-3. go to push management 
-4. go to push template
-5. go to add new template
-6. try to check with empty text in the template name field</t>
-  </si>
-  <si>
     <t>an error message will show "please enter no more than 100 characters."</t>
   </si>
   <si>
@@ -267,13 +259,13 @@
     <t>SYM-AP_APT_IU_026</t>
   </si>
   <si>
-    <t>input a valid image url from a well-known source (e.g., Unsplash) and ensure it loads correctly</t>
-  </si>
-  <si>
     <t>input an invalid url and verify that the system handles it gracefully, displaying an appropriate error message.</t>
   </si>
   <si>
     <t>submit the form with an empty Image URL field and check if the system prompts for a required field</t>
+  </si>
+  <si>
+    <t>input a valid image URL from a well-known source (e.g., Unsplash) and ensure it loads correctly in the image URL field</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1362,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1387,7 +1379,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1487,16 +1479,16 @@
     </row>
     <row r="4" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>9</v>
@@ -1529,13 +1521,13 @@
     </row>
     <row r="5" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>10</v>
@@ -1567,19 +1559,19 @@
     </row>
     <row r="6" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1605,19 +1597,19 @@
     </row>
     <row r="7" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1643,7 +1635,7 @@
     </row>
     <row r="8" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>40</v>
@@ -1681,7 +1673,7 @@
     </row>
     <row r="9" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>40</v>
@@ -1719,7 +1711,7 @@
     </row>
     <row r="10" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>40</v>
@@ -1757,7 +1749,7 @@
     </row>
     <row r="11" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>40</v>
@@ -1795,7 +1787,7 @@
     </row>
     <row r="12" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>40</v>
@@ -1833,7 +1825,7 @@
     </row>
     <row r="13" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>40</v>
@@ -1871,7 +1863,7 @@
     </row>
     <row r="14" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>40</v>
@@ -1909,7 +1901,7 @@
     </row>
     <row r="15" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>40</v>
@@ -1947,7 +1939,7 @@
     </row>
     <row r="16" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>40</v>
@@ -1985,7 +1977,7 @@
     </row>
     <row r="17" spans="1:26" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>40</v>
@@ -2023,7 +2015,7 @@
     </row>
     <row r="18" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>40</v>
@@ -2061,7 +2053,7 @@
     </row>
     <row r="19" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>40</v>
@@ -2099,7 +2091,7 @@
     </row>
     <row r="20" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>40</v>
@@ -2137,7 +2129,7 @@
     </row>
     <row r="21" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>40</v>
@@ -2175,7 +2167,7 @@
     </row>
     <row r="22" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>40</v>
@@ -2213,7 +2205,7 @@
     </row>
     <row r="23" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>40</v>
@@ -2251,7 +2243,7 @@
     </row>
     <row r="24" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>40</v>
@@ -2289,7 +2281,7 @@
     </row>
     <row r="25" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>40</v>
@@ -2327,7 +2319,7 @@
     </row>
     <row r="26" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>40</v>
@@ -2365,7 +2357,7 @@
     </row>
     <row r="27" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>40</v>
@@ -2403,7 +2395,7 @@
     </row>
     <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>40</v>
@@ -2441,7 +2433,7 @@
     </row>
     <row r="29" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>40</v>

</xml_diff>